<commit_message>
- BC nhomHoTro: fix err export excel 'colspan' & sum in excel
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoNhomHoTro.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoNhomHoTro.xlsx
@@ -546,11 +546,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D23" sqref="D23"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,27 +886,41 @@
       <c r="H28" s="7"/>
       <c r="I28" s="14"/>
     </row>
-    <row r="29" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="19" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="14"/>
+    </row>
+    <row r="30" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B29" s="20"/>
-      <c r="C29" s="20"/>
-      <c r="D29" s="20"/>
-      <c r="E29" s="9">
-        <f>SUM(E$5:E28)</f>
+      <c r="B30" s="20"/>
+      <c r="C30" s="20"/>
+      <c r="D30" s="20"/>
+      <c r="E30" s="9">
+        <f>SUM(E$5:E29)</f>
         <v>0</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="13"/>
+      <c r="F30" s="16"/>
+      <c r="G30" s="16">
+        <f>SUM(G$5:G29)</f>
+        <v>0</v>
+      </c>
+      <c r="H30" s="16"/>
+      <c r="I30" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A29:D29"/>
+    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
temp export: xoa cot TongCong
</commit_message>
<xml_diff>
--- a/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoNhomHoTro.xlsx
+++ b/banhang24/Template/ExportExcel/Report/BaoCaoKho/Teamplate_BaoCaoNhomHoTro.xlsx
@@ -17,10 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Tổng cộng:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Mã khách hàng</t>
   </si>
@@ -99,7 +96,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -111,14 +108,8 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -141,49 +132,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -207,9 +161,6 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -218,28 +169,16 @@
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -546,11 +485,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,64 +501,64 @@
     <col min="5" max="5" width="32.85546875" style="8" customWidth="1"/>
     <col min="6" max="6" width="23.140625" style="8" customWidth="1"/>
     <col min="7" max="7" width="23" style="8" customWidth="1"/>
-    <col min="8" max="8" width="23" style="12" customWidth="1"/>
+    <col min="8" max="8" width="23" style="11" customWidth="1"/>
     <col min="9" max="9" width="19.7109375" style="1" customWidth="1"/>
     <col min="10" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="17" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
+      <c r="A1" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
       <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="10"/>
+      <c r="A3" s="9"/>
     </row>
     <row r="4" spans="1:9" s="6" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="F4" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="G4" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="10" t="s">
         <v>9</v>
-      </c>
-      <c r="F4" s="15" t="s">
-        <v>5</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>6</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" s="11" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
@@ -631,7 +570,7 @@
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
       <c r="H5" s="7"/>
-      <c r="I5" s="14"/>
+      <c r="I5" s="12"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="4"/>
@@ -642,7 +581,7 @@
       <c r="F6" s="7"/>
       <c r="G6" s="7"/>
       <c r="H6" s="7"/>
-      <c r="I6" s="14"/>
+      <c r="I6" s="12"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
@@ -653,7 +592,7 @@
       <c r="F7" s="7"/>
       <c r="G7" s="7"/>
       <c r="H7" s="7"/>
-      <c r="I7" s="14"/>
+      <c r="I7" s="12"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -664,7 +603,7 @@
       <c r="F8" s="7"/>
       <c r="G8" s="7"/>
       <c r="H8" s="7"/>
-      <c r="I8" s="14"/>
+      <c r="I8" s="12"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
@@ -675,7 +614,7 @@
       <c r="F9" s="7"/>
       <c r="G9" s="7"/>
       <c r="H9" s="7"/>
-      <c r="I9" s="14"/>
+      <c r="I9" s="12"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
@@ -686,7 +625,7 @@
       <c r="F10" s="7"/>
       <c r="G10" s="7"/>
       <c r="H10" s="7"/>
-      <c r="I10" s="14"/>
+      <c r="I10" s="12"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
@@ -697,7 +636,7 @@
       <c r="F11" s="7"/>
       <c r="G11" s="7"/>
       <c r="H11" s="7"/>
-      <c r="I11" s="14"/>
+      <c r="I11" s="12"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
@@ -708,7 +647,7 @@
       <c r="F12" s="7"/>
       <c r="G12" s="7"/>
       <c r="H12" s="7"/>
-      <c r="I12" s="14"/>
+      <c r="I12" s="12"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
@@ -719,7 +658,7 @@
       <c r="F13" s="7"/>
       <c r="G13" s="7"/>
       <c r="H13" s="7"/>
-      <c r="I13" s="14"/>
+      <c r="I13" s="12"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
@@ -730,7 +669,7 @@
       <c r="F14" s="7"/>
       <c r="G14" s="7"/>
       <c r="H14" s="7"/>
-      <c r="I14" s="14"/>
+      <c r="I14" s="12"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
@@ -741,7 +680,7 @@
       <c r="F15" s="7"/>
       <c r="G15" s="7"/>
       <c r="H15" s="7"/>
-      <c r="I15" s="14"/>
+      <c r="I15" s="12"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
@@ -752,7 +691,7 @@
       <c r="F16" s="7"/>
       <c r="G16" s="7"/>
       <c r="H16" s="7"/>
-      <c r="I16" s="14"/>
+      <c r="I16" s="12"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
@@ -763,7 +702,7 @@
       <c r="F17" s="7"/>
       <c r="G17" s="7"/>
       <c r="H17" s="7"/>
-      <c r="I17" s="14"/>
+      <c r="I17" s="12"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
@@ -774,7 +713,7 @@
       <c r="F18" s="7"/>
       <c r="G18" s="7"/>
       <c r="H18" s="7"/>
-      <c r="I18" s="14"/>
+      <c r="I18" s="12"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
@@ -785,7 +724,7 @@
       <c r="F19" s="7"/>
       <c r="G19" s="7"/>
       <c r="H19" s="7"/>
-      <c r="I19" s="14"/>
+      <c r="I19" s="12"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
@@ -796,7 +735,7 @@
       <c r="F20" s="7"/>
       <c r="G20" s="7"/>
       <c r="H20" s="7"/>
-      <c r="I20" s="14"/>
+      <c r="I20" s="12"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
@@ -807,7 +746,7 @@
       <c r="F21" s="7"/>
       <c r="G21" s="7"/>
       <c r="H21" s="7"/>
-      <c r="I21" s="14"/>
+      <c r="I21" s="12"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
@@ -818,7 +757,7 @@
       <c r="F22" s="7"/>
       <c r="G22" s="7"/>
       <c r="H22" s="7"/>
-      <c r="I22" s="14"/>
+      <c r="I22" s="12"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
@@ -829,7 +768,7 @@
       <c r="F23" s="7"/>
       <c r="G23" s="7"/>
       <c r="H23" s="7"/>
-      <c r="I23" s="14"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
@@ -840,7 +779,7 @@
       <c r="F24" s="7"/>
       <c r="G24" s="7"/>
       <c r="H24" s="7"/>
-      <c r="I24" s="14"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
@@ -851,7 +790,7 @@
       <c r="F25" s="7"/>
       <c r="G25" s="7"/>
       <c r="H25" s="7"/>
-      <c r="I25" s="14"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
@@ -862,7 +801,7 @@
       <c r="F26" s="7"/>
       <c r="G26" s="7"/>
       <c r="H26" s="7"/>
-      <c r="I26" s="14"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
@@ -873,7 +812,7 @@
       <c r="F27" s="7"/>
       <c r="G27" s="7"/>
       <c r="H27" s="7"/>
-      <c r="I27" s="14"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
@@ -884,7 +823,7 @@
       <c r="F28" s="7"/>
       <c r="G28" s="7"/>
       <c r="H28" s="7"/>
-      <c r="I28" s="14"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
@@ -895,32 +834,12 @@
       <c r="F29" s="7"/>
       <c r="G29" s="7"/>
       <c r="H29" s="7"/>
-      <c r="I29" s="14"/>
-    </row>
-    <row r="30" spans="1:9" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30" s="20"/>
-      <c r="C30" s="20"/>
-      <c r="D30" s="20"/>
-      <c r="E30" s="9">
-        <f>SUM(E$5:E29)</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16">
-        <f>SUM(G$5:G29)</f>
-        <v>0</v>
-      </c>
-      <c r="H30" s="16"/>
-      <c r="I30" s="13"/>
+      <c r="I29" s="12"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="2">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="A2:H2"/>
-    <mergeCell ref="A30:D30"/>
   </mergeCells>
   <pageMargins left="0.76" right="0.23" top="0.78" bottom="0.87" header="0.3" footer="0.7"/>
   <pageSetup scale="95" orientation="landscape" r:id="rId1"/>

</xml_diff>